<commit_message>
Round Trip Engagement changes - Mid - 21 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEA573F6-CFC9-49A0-BDEC-DC491EED9F57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F2420-686B-4993-87B9-0FE823E4F292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="92">
   <si>
     <t>Subject</t>
   </si>
@@ -265,12 +265,6 @@
     <t>An engagement is typically considered a potential round trip if it is acquired by a sponsor (subject is a potential round trip) or by a sponsor-backed operating company (buyer is a potential round trip). Note "sponsor" includes firms tagged as Private Equity Group, Hedge Fund, or Family Office.</t>
   </si>
   <si>
-    <t>TPG Global, LLC</t>
-  </si>
-  <si>
-    <t>Poundworld Retail Ltd.</t>
-  </si>
-  <si>
     <t>Private Equity Group</t>
   </si>
   <si>
@@ -292,12 +286,6 @@
     <t>Client Potential Round Trip</t>
   </si>
   <si>
-    <t>Pharmavite, LLC</t>
-  </si>
-  <si>
-    <t>Food State, Inc.</t>
-  </si>
-  <si>
     <t>Hedge Fund</t>
   </si>
   <si>
@@ -319,25 +307,19 @@
     <t>Change Company Type</t>
   </si>
   <si>
-    <t>Team, Inc</t>
-  </si>
-  <si>
-    <t>QualSpec Group</t>
-  </si>
-  <si>
     <t>Private Equity</t>
   </si>
   <si>
     <t>Giselle Segura</t>
   </si>
   <si>
-    <t>EagleBank</t>
-  </si>
-  <si>
-    <t>Eagle Bancorp, inc</t>
-  </si>
-  <si>
     <t>CF Cao User</t>
+  </si>
+  <si>
+    <t>Grupo Volum</t>
+  </si>
+  <si>
+    <t>GPF Capital</t>
   </si>
 </sst>
 </file>
@@ -688,7 +670,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -703,7 +685,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +693,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>
@@ -843,12 +825,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -860,8 +842,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -969,10 +951,10 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>73</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
-        <v>74</v>
+        <v>90</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1011,19 +993,19 @@
         <v>66</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="S2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>44</v>
@@ -1047,10 +1029,10 @@
         <v>50</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AC2" t="s">
         <v>66</v>
@@ -1060,12 +1042,6 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B3" t="s">
-        <v>83</v>
-      </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
@@ -1103,19 +1079,19 @@
         <v>66</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="S3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>44</v>
@@ -1139,10 +1115,10 @@
         <v>50</v>
       </c>
       <c r="AA3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB3" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AC3" t="s">
         <v>66</v>
@@ -1152,12 +1128,6 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B4" t="s">
-        <v>92</v>
-      </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
@@ -1195,19 +1165,19 @@
         <v>66</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R4" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="S4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T4" s="3" t="s">
         <v>44</v>
@@ -1231,10 +1201,10 @@
         <v>50</v>
       </c>
       <c r="AA4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB4" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AC4" t="s">
         <v>66</v>
@@ -1244,12 +1214,6 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
       <c r="C5" t="s">
         <v>37</v>
       </c>
@@ -1287,19 +1251,19 @@
         <v>66</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="R5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="S5" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="T5" s="3" t="s">
         <v>44</v>
@@ -1323,10 +1287,10 @@
         <v>50</v>
       </c>
       <c r="AA5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AB5" s="3" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="AC5" t="s">
         <v>66</v>
@@ -1345,7 +1309,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1357,57 +1321,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C2" t="s">
         <v>51</v>
-      </c>
-      <c r="B2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" t="s">
         <v>51</v>
-      </c>
-      <c r="B3" t="s">
-        <v>79</v>
-      </c>
-      <c r="C3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B4" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
         <v>51</v>
-      </c>
-      <c r="B4" t="s">
-        <v>79</v>
-      </c>
-      <c r="C4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C5" t="s">
         <v>51</v>
-      </c>
-      <c r="B5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C5" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1498,18 +1462,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Round Trip (subjct) - Final - 21 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A3F2420-686B-4993-87B9-0FE823E4F292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A443ACBE-D19C-49B8-ABB3-CD1877F41A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="98">
   <si>
     <t>Subject</t>
   </si>
@@ -307,9 +307,6 @@
     <t>Change Company Type</t>
   </si>
   <si>
-    <t>Private Equity</t>
-  </si>
-  <si>
     <t>Giselle Segura</t>
   </si>
   <si>
@@ -320,6 +317,27 @@
   </si>
   <si>
     <t>GPF Capital</t>
+  </si>
+  <si>
+    <t>Public Equity</t>
+  </si>
+  <si>
+    <t>Owl Wire and Cable LLC</t>
+  </si>
+  <si>
+    <t>International Wire Group, Inc.</t>
+  </si>
+  <si>
+    <t>3i Group Plc</t>
+  </si>
+  <si>
+    <t>IRISNDT Corp.</t>
+  </si>
+  <si>
+    <t>Mirait Holdings Corporation</t>
+  </si>
+  <si>
+    <t>Seibu Construction Co., Ltd.</t>
   </si>
 </sst>
 </file>
@@ -685,7 +703,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -693,7 +711,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
   </sheetData>
@@ -843,13 +861,13 @@
   <dimension ref="A1:AD5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="21.77734375" customWidth="1"/>
+    <col min="1" max="1" width="25.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.77734375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="22.88671875" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="17.77734375" bestFit="1" customWidth="1"/>
@@ -951,10 +969,10 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1042,6 +1060,12 @@
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>92</v>
+      </c>
       <c r="C3" t="s">
         <v>37</v>
       </c>
@@ -1128,6 +1152,12 @@
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" t="s">
+        <v>95</v>
+      </c>
       <c r="C4" t="s">
         <v>37</v>
       </c>
@@ -1174,7 +1204,7 @@
         <v>75</v>
       </c>
       <c r="R4" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="S4" t="s">
         <v>74</v>
@@ -1214,6 +1244,12 @@
       </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
       <c r="C5" t="s">
         <v>37</v>
       </c>
@@ -1260,7 +1296,7 @@
         <v>75</v>
       </c>
       <c r="R5" t="s">
-        <v>87</v>
+        <v>91</v>
       </c>
       <c r="S5" t="s">
         <v>74</v>

</xml_diff>

<commit_message>
TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip - Initial Complete - 26 May 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A443ACBE-D19C-49B8-ABB3-CD1877F41A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555CFBC2-1CAC-47E2-82CF-D9F2B826EAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -292,9 +292,6 @@
     <t>Warning Msg</t>
   </si>
   <si>
-    <t>A Subject is typically considered a potential round trip if it is an operating company acquired either by a Private Equity firm or by a PE-owned operating company. The Subject is not listed as an Operating Company. If you still want to consider them a round trip candidate no change is needed; otherwise, please change the selection.</t>
-  </si>
-  <si>
     <t>Reason</t>
   </si>
   <si>
@@ -338,6 +335,9 @@
   </si>
   <si>
     <t>Seibu Construction Co., Ltd.</t>
+  </si>
+  <si>
+    <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
 </sst>
 </file>
@@ -703,7 +703,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -711,7 +711,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
   </sheetData>
@@ -832,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -846,9 +846,9 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -860,7 +860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1175537-D85E-4D33-8AD2-B3C163BE409D}">
   <dimension ref="A1:AD5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
@@ -969,10 +969,10 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1061,10 +1061,10 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -1153,10 +1153,10 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>93</v>
+      </c>
+      <c r="B4" t="s">
         <v>94</v>
-      </c>
-      <c r="B4" t="s">
-        <v>95</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -1204,7 +1204,7 @@
         <v>75</v>
       </c>
       <c r="R4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S4" t="s">
         <v>74</v>
@@ -1245,10 +1245,10 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" t="s">
         <v>96</v>
-      </c>
-      <c r="B5" t="s">
-        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -1296,7 +1296,7 @@
         <v>75</v>
       </c>
       <c r="R5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="S5" t="s">
         <v>74</v>
@@ -1498,18 +1498,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Initial - TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip - 2nd June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{555CFBC2-1CAC-47E2-82CF-D9F2B826EAE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79726645-5C3D-4632-B90D-426F36E93E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -337,7 +337,7 @@
     <t>Seibu Construction Co., Ltd.</t>
   </si>
   <si>
-    <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
+    <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Subject is not listed as an Operating Company. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
 </sst>
 </file>
@@ -410,7 +410,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -830,15 +841,16 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="67.88671875" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
@@ -846,12 +858,18 @@
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
         <v>97</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" s="4"/>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A4 A2">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Mid - 02 June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79726645-5C3D-4632-B90D-426F36E93E3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09FB56E-A3DD-47BC-BE4B-750140063D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="102">
   <si>
     <t>Subject</t>
   </si>
@@ -298,9 +298,6 @@
     <t>Comment</t>
   </si>
   <si>
-    <t>Requesting to change Company Type to Operating Company because it is being considered to be a potential round trip</t>
-  </si>
-  <si>
     <t>Change Company Type</t>
   </si>
   <si>
@@ -338,6 +335,21 @@
   </si>
   <si>
     <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Subject is not listed as an Operating Company. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Warning Msg 2</t>
+  </si>
+  <si>
+    <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to Operating Company and Ownership to Private Equity Group because it is being considered to be a potential round trip</t>
+  </si>
+  <si>
+    <t>Warning Msg 3</t>
+  </si>
+  <si>
+    <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round-trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
 </sst>
 </file>
@@ -714,7 +726,7 @@
         <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -722,7 +734,7 @@
         <v>66</v>
       </c>
       <c r="B2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -841,29 +853,42 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="67.88671875" customWidth="1"/>
+    <col min="2" max="3" width="57.6640625" customWidth="1"/>
     <col min="4" max="4" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" ht="72" x14ac:dyDescent="0.3">
+      <c r="B1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+        <v>96</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="4"/>
     </row>
   </sheetData>
@@ -987,10 +1012,10 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C2" t="s">
         <v>37</v>
@@ -1079,10 +1104,10 @@
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C3" t="s">
         <v>37</v>
@@ -1171,10 +1196,10 @@
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B4" t="s">
         <v>93</v>
-      </c>
-      <c r="B4" t="s">
-        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>37</v>
@@ -1222,7 +1247,7 @@
         <v>75</v>
       </c>
       <c r="R4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S4" t="s">
         <v>74</v>
@@ -1263,10 +1288,10 @@
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" t="s">
-        <v>96</v>
       </c>
       <c r="C5" t="s">
         <v>37</v>
@@ -1314,7 +1339,7 @@
         <v>75</v>
       </c>
       <c r="R5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="S5" t="s">
         <v>74</v>
@@ -1505,7 +1530,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="B11" sqref="B10:B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1522,12 +1547,12 @@
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Mid Day (New) - 2 June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B09FB56E-A3DD-47BC-BE4B-750140063D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557B0EA1-7A10-4EA2-9EA3-2D574816B134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
     <t>Warning Msg 3</t>
   </si>
   <si>
-    <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round-trip candidate no change is needed; otherwise, please change the selection.</t>
+    <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Added - TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_NeitherSubjectNorBuyerIsAPotentialRoundTrip - 2nd June 2025
</commit_message>
<xml_diff>
--- a/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
+++ b/TestData/TMTT0046984_VerificationOfEngCompanyRoundtripFlagFunctionalityOnTheBuysideDeals_BuyerIsAPotentialRoundTrip.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SMittal0207\source\repos\SF_Automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557B0EA1-7A10-4EA2-9EA3-2D574816B134}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89C32175-9424-4F49-9482-2E7F1ACBD177}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="568" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="2" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="106">
   <si>
     <t>Subject</t>
   </si>
@@ -350,6 +350,18 @@
   </si>
   <si>
     <t>A Buyer is typically only considered a potential round trip if it is a private equity-owned operating company that has acquired and fully absorbed the Subject operating company. The Subject is not listed as an Operating Company AND the Buyer is not listed as an Operating Company with Private Equity/Hedge Fund/Family Office ownership. If you still want to consider the Buyer a round trip candidate no change is needed; otherwise, please change the selection.</t>
+  </si>
+  <si>
+    <t>Comment 2</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to Operating Company with Ownership: Private Equity Group because it is being considered to be a potential round trip</t>
+  </si>
+  <si>
+    <t>Requesting to change Company Type to Operating Company because it is being considered to be a potential round trip</t>
+  </si>
+  <si>
+    <t>Comment 3</t>
   </si>
 </sst>
 </file>
@@ -855,7 +867,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{428EFC0A-BA50-4449-A054-B06ABB328678}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -1527,32 +1539,45 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92EA0090-8A70-4EE9-9BBD-D73C51089E4F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B10:B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.44140625" customWidth="1"/>
-    <col min="2" max="2" width="56" customWidth="1"/>
+    <col min="2" max="3" width="56" customWidth="1"/>
+    <col min="4" max="4" width="47.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
         <v>82</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="C1" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="9" t="s">
         <v>99</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>103</v>
       </c>
     </row>
   </sheetData>

</xml_diff>